<commit_message>
Cleaning and documenting the workflow, extracting the missing denisty plots
</commit_message>
<xml_diff>
--- a/inventory_global_products.xlsx
+++ b/inventory_global_products.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sputnik/Documents/Natural_capital/NBS_OP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01923D05-C824-0A43-89A9-619376373DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C37690-8452-9244-9BD1-5B2E0CF3EB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{FE3DF1B3-9048-0645-9424-76FF919EF56D}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{FE3DF1B3-9048-0645-9424-76FF919EF56D}"/>
   </bookViews>
   <sheets>
     <sheet name="inventory_global_products" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="558">
   <si>
     <t>Scenario</t>
   </si>
@@ -1688,13 +1689,19 @@
   </si>
   <si>
     <t>NBSdiff_sed_export_2020-reforest2_compressed_md5_ff25f0.tif</t>
+  </si>
+  <si>
+    <t>Conservation</t>
+  </si>
+  <si>
+    <t>si</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1827,6 +1834,13 @@
       <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2171,8 +2185,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2550,8 +2565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C036149-30B1-CB4A-9539-0B493FA5906D}">
   <dimension ref="A1:K219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3081,7 +3096,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C20" t="s">
@@ -3107,7 +3122,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C21" t="s">
@@ -3133,7 +3148,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C22" t="s">
@@ -3159,7 +3174,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C23" t="s">
@@ -3185,7 +3200,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C24" t="s">
@@ -7759,6 +7774,655 @@
       </c>
       <c r="G219" t="s">
         <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976F0BBF-6E1C-F84C-A5DE-45D3CC2FF64A}">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="36.5" customWidth="1"/>
+    <col min="6" max="6" width="104.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>556</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>556</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3">
+        <v>2020</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>556</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>2020</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>556</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>2020</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>556</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>2017</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16">
+        <v>2017</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17">
+        <v>2019</v>
+      </c>
+      <c r="E17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18">
+        <v>2019</v>
+      </c>
+      <c r="E18" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>2019</v>
+      </c>
+      <c r="E19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>95</v>
+      </c>
+      <c r="G22" t="s">
+        <v>88</v>
+      </c>
+      <c r="H22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Have to check the calcvualtion of the shares to see what happend there. Get the data with the updated restoration areas and re do this. Add access and coastal risk protection
</commit_message>
<xml_diff>
--- a/inventory_global_products.xlsx
+++ b/inventory_global_products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sputnik/Documents/Natural_capital/NBS_OP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C37690-8452-9244-9BD1-5B2E0CF3EB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39446EFD-0203-C24B-A0BF-C36A02D7FD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{FE3DF1B3-9048-0645-9424-76FF919EF56D}"/>
+    <workbookView xWindow="4000" yWindow="3000" windowWidth="25600" windowHeight="15500" xr2:uid="{FE3DF1B3-9048-0645-9424-76FF919EF56D}"/>
   </bookViews>
   <sheets>
     <sheet name="inventory_global_products" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="559">
   <si>
     <t>Scenario</t>
   </si>
@@ -1695,6 +1695,9 @@
   </si>
   <si>
     <t>si</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2565,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C036149-30B1-CB4A-9539-0B493FA5906D}">
   <dimension ref="A1:K219"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7783,10 +7786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976F0BBF-6E1C-F84C-A5DE-45D3CC2FF64A}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="C6" zoomScale="135" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8425,6 +8428,11 @@
         <v>89</v>
       </c>
     </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>558</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaning old files not necessary anymore. Preparing to split into global natcap and nbs_op
</commit_message>
<xml_diff>
--- a/inventory_global_products.xlsx
+++ b/inventory_global_products.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldwildlifefund-my.sharepoint.com/personal/jeronimo_rodriguez_wwfus_org/Documents/NBS_op/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodriguez/NBSOp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="338" documentId="13_ncr:1_{39446EFD-0203-C24B-A0BF-C36A02D7FD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8353D525-EB5B-BA47-9D95-AFC8DA9EFA76}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C3BC84C-D221-6643-A43B-95071733ED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FE3DF1B3-9048-0645-9424-76FF919EF56D}"/>
+    <workbookView xWindow="1960" yWindow="500" windowWidth="20960" windowHeight="19640" activeTab="2" xr2:uid="{FE3DF1B3-9048-0645-9424-76FF919EF56D}"/>
   </bookViews>
   <sheets>
     <sheet name="inventory_global_products" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="Initial Exploration" sheetId="2" r:id="rId2"/>
+    <sheet name="Scratch" sheetId="4" r:id="rId3"/>
+    <sheet name="Band LC_ESA" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">inventory_global_products!$A$1:$K$219</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="575">
   <si>
     <t>Scenario</t>
   </si>
@@ -1751,314 +1751,29 @@
     <t>ton/ha/year</t>
   </si>
   <si>
-    <t>AGU Sessions</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/233716</t>
-  </si>
-  <si>
-    <t>GC41B - Earth Observation–Based Methods to Monitor Forest Loss, Degradation, and Growth I Oral</t>
-  </si>
-  <si>
-    <t>8:30-10:00</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/240425</t>
-  </si>
-  <si>
-    <t>SY41A - Advancing Socioeconomic Impact and Resource Sustainability Through Earth Observations: Using Integrated EO for Informed Decision-Making Leading to Economic Benefits, Emphasizing Partly the Water, Food, and Energy Nexus I Oral</t>
-  </si>
-  <si>
-    <t>Mabel</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/233446</t>
-  </si>
-  <si>
-    <t>GC44F - Advancing Understanding of the Impacts of Land Use and Land Cover Changes in Climate Modeling II eLightning</t>
-  </si>
-  <si>
-    <t>13:00-17:30</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/233727</t>
-  </si>
-  <si>
-    <t>GC44B - Earth Observation–Based Methods to Monitor Forest Loss, Degradation, and Growth II Oral</t>
-  </si>
-  <si>
-    <t>16:00-17:30</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/233359</t>
-  </si>
-  <si>
-    <t>GC51C - Advancing Climate-Smart Agriculture: From Assessing Risks to Implementing Sustainable Adaptation I Oral</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/234080</t>
-  </si>
-  <si>
-    <t>GC51E - Robustness of Climate Change Information for Decisions I Oral</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/225240</t>
-  </si>
-  <si>
-    <t>GC51K - Advancing Sustainable Agriculture: Integrating AI, Machine Learning, and Deep Learning Poster</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/228797</t>
-  </si>
-  <si>
-    <t>GC51N - Earth Observation–Based Methods to Monitor Forest Loss, Degradation, and Growth III Poster</t>
-  </si>
-  <si>
-    <t>Poster 8:30-12</t>
-  </si>
-  <si>
-    <t>GC51W - Sustainable Agriculture and Climate Change: Toward Agricultural Decarbonization I Poster</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/233926</t>
-  </si>
-  <si>
-    <t>GC52D - Multisector Dynamics: Advances in Global-to-Regional Land Use and Land Cover Change Modeling II Oral</t>
-  </si>
-  <si>
-    <t>10:20-11:50</t>
-  </si>
-  <si>
-    <t>!!!!!!</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/233756</t>
-  </si>
-  <si>
-    <t>GC53K - Forest Cover Dynamics, Drivers, and Impacts Under Diverse Human Activities and Climate Change II Oral</t>
-  </si>
-  <si>
-    <t>14:10-15:40</t>
-  </si>
-  <si>
-    <t>https://agu.confex.com/agu/agu24/meetingapp.cgi/Session/234166</t>
-  </si>
-  <si>
-    <t>GC54E - Science Goals, Measurement Needs, and Technical Advances Toward Achieving NASA’s Surface Topography and Vegetation Targeted Observable II Oral</t>
-  </si>
-  <si>
-    <t>* if something</t>
-  </si>
-  <si>
-    <t>Global Nat Cap</t>
-  </si>
-  <si>
-    <t>Dataset Name</t>
-  </si>
-  <si>
-    <t>Timeframe</t>
-  </si>
-  <si>
-    <t>Frequency</t>
-  </si>
-  <si>
-    <t>Spatial Resolution</t>
-  </si>
-  <si>
-    <t>Classification Scheme</t>
-  </si>
-  <si>
-    <t>Reported Accuracy</t>
-  </si>
-  <si>
-    <t>Input Data Sources</t>
-  </si>
-  <si>
-    <t>MODIS Land Cover (MCD12Q1)</t>
-  </si>
-  <si>
-    <t>2001–Present</t>
-  </si>
-  <si>
-    <t>Annual</t>
-  </si>
-  <si>
-    <t>500 m</t>
-  </si>
-  <si>
-    <t>17 classes (IGBP scheme)</t>
-  </si>
-  <si>
-    <t>~75% overall</t>
-  </si>
-  <si>
-    <t>MODIS satellite imagery</t>
-  </si>
-  <si>
-    <t>ESA Climate Change Initiative Land Cover (CCI-LC)</t>
-  </si>
-  <si>
-    <t>1992–2015</t>
-  </si>
-  <si>
-    <t>300 m</t>
-  </si>
-  <si>
-    <t>22 classes (UN LCCS)</t>
-  </si>
-  <si>
-    <t>~71% overall</t>
-  </si>
-  <si>
-    <t>MERIS, AVHRR, SPOT-VGT, PROBA-V, and other satellite data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exclude </t>
-  </si>
-  <si>
-    <t>iso3</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>GlobeLand30</t>
-  </si>
-  <si>
-    <t>2000, 2010, 2020</t>
-  </si>
-  <si>
-    <t>Decadal</t>
-  </si>
-  <si>
-    <t>30 m</t>
-  </si>
-  <si>
-    <t>10 classes</t>
-  </si>
-  <si>
-    <t>~80% overall</t>
-  </si>
-  <si>
-    <t>Landsat TM/ETM+, HJ-1 satellite imagery</t>
-  </si>
-  <si>
-    <t>ATA</t>
-  </si>
-  <si>
-    <t>Antarctica</t>
-  </si>
-  <si>
-    <t>Dynamic World (DW)</t>
-  </si>
-  <si>
-    <t>2020–Present</t>
-  </si>
-  <si>
-    <t>Near Real-Time</t>
-  </si>
-  <si>
-    <t>10 m</t>
-  </si>
-  <si>
-    <t>9 classes</t>
-  </si>
-  <si>
-    <t>~72% overall</t>
-  </si>
-  <si>
-    <t>Sentinel-2 imagery</t>
-  </si>
-  <si>
-    <t>FRO</t>
-  </si>
-  <si>
-    <t>Faroe Islands</t>
-  </si>
-  <si>
-    <t>ESA WorldCover (WC)</t>
-  </si>
-  <si>
-    <t>11 classes</t>
-  </si>
-  <si>
-    <t>~65% overall</t>
-  </si>
-  <si>
-    <t>Sentinel-1 and Sentinel-2 imagery</t>
-  </si>
-  <si>
-    <t>ISL</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Esri Land Cover (Esri)</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>FROM-GLC</t>
-  </si>
-  <si>
-    <t>One-time</t>
-  </si>
-  <si>
-    <t>~64.9% overall</t>
-  </si>
-  <si>
-    <t>Landsat imagery</t>
-  </si>
-  <si>
-    <t>GRL</t>
-  </si>
-  <si>
-    <t>Greenland</t>
-  </si>
-  <si>
-    <t>Tsinghua University Land Cover</t>
-  </si>
-  <si>
-    <t>1985–2020</t>
-  </si>
-  <si>
-    <t>33 classes</t>
-  </si>
-  <si>
-    <t>~80% (Level 1); ~73% (Level 2)</t>
-  </si>
-  <si>
-    <t>Landsat TM/ETM+, domestic high-resolution satellite data, Planet imagery </t>
-  </si>
-  <si>
-    <t>NOR</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Z:\bck_archive\move to swy-global\global_dem_3s_md5_22d0c3809af491fa09d03002bdf09748</t>
-  </si>
-  <si>
-    <t>Z:\bigboi_freefilesync_backup\repositories\ndr_sdr_global\data\watersheds_globe_HydroSHEDS_15arcseconds_md5_c6acf2762123bbd5de605358e733a304</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: </t>
+  </si>
+  <si>
+    <t>'/home/jeronimo/global_ES_modeling/esos-c/data/ndr/ESA_LC/ESACCI-LC-L4-LCCS-Map-300m-P1Y-1992_2015-v2.0.7.tif'</t>
+  </si>
+  <si>
+    <t>Band</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2207,27 +1922,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2593,19 +2287,13 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2985,16 +2673,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K219"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="A239" sqref="A239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="73.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="4" max="4" width="30.6640625" customWidth="1"/>
     <col min="5" max="5" width="71.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3132,8 +2820,11 @@
       <c r="F6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3175,6 +2866,9 @@
       <c r="F8" t="s">
         <v>15</v>
       </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -3315,6 +3009,9 @@
       <c r="F15" t="s">
         <v>15</v>
       </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -3335,6 +3032,9 @@
       <c r="F16" t="s">
         <v>15</v>
       </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -3767,6 +3467,9 @@
       <c r="F37" t="s">
         <v>116</v>
       </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -3807,6 +3510,9 @@
       <c r="F39" t="s">
         <v>116</v>
       </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -3947,6 +3653,9 @@
       <c r="F46" t="s">
         <v>116</v>
       </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -4087,6 +3796,9 @@
       <c r="F53" t="s">
         <v>15</v>
       </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -4107,6 +3819,9 @@
       <c r="F54" t="s">
         <v>15</v>
       </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -4320,7 +4035,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -4339,8 +4054,11 @@
       <c r="F65" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>440</v>
       </c>
@@ -4360,7 +4078,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>227</v>
       </c>
@@ -4380,7 +4098,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>230</v>
       </c>
@@ -4400,7 +4118,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>167</v>
       </c>
@@ -4420,7 +4138,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -4440,7 +4158,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>387</v>
       </c>
@@ -4460,7 +4178,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>466</v>
       </c>
@@ -4480,7 +4198,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>34</v>
       </c>
@@ -4499,8 +4217,11 @@
       <c r="F73" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G73">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -4519,8 +4240,11 @@
       <c r="F74" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -4539,8 +4263,11 @@
       <c r="F75" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>440</v>
       </c>
@@ -4560,7 +4287,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>227</v>
       </c>
@@ -4580,7 +4307,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>230</v>
       </c>
@@ -4600,7 +4327,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>167</v>
       </c>
@@ -4620,7 +4347,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>167</v>
       </c>
@@ -4908,6 +4635,9 @@
       <c r="F93" t="s">
         <v>15</v>
       </c>
+      <c r="G93">
+        <v>5</v>
+      </c>
     </row>
     <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -4928,6 +4658,9 @@
       <c r="F94" t="s">
         <v>15</v>
       </c>
+      <c r="G94">
+        <v>5</v>
+      </c>
     </row>
     <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
@@ -4969,7 +4702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>11</v>
       </c>
@@ -5177,6 +4910,9 @@
       <c r="F106" t="s">
         <v>15</v>
       </c>
+      <c r="G106">
+        <v>5</v>
+      </c>
     </row>
     <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
@@ -5197,6 +4933,9 @@
       <c r="F107" t="s">
         <v>15</v>
       </c>
+      <c r="G107">
+        <v>5</v>
+      </c>
     </row>
     <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
@@ -5266,8 +5005,11 @@
       <c r="F110" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G110">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>11</v>
       </c>
@@ -6190,6 +5932,9 @@
       <c r="F155" t="s">
         <v>15</v>
       </c>
+      <c r="G155">
+        <v>5</v>
+      </c>
     </row>
     <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
@@ -6355,7 +6100,7 @@
       <c r="A164" t="s">
         <v>387</v>
       </c>
-      <c r="B164" s="6" t="s">
+      <c r="B164" s="5" t="s">
         <v>197</v>
       </c>
       <c r="C164" t="s">
@@ -6714,7 +6459,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>11</v>
       </c>
@@ -6756,6 +6501,9 @@
       <c r="F180" t="s">
         <v>15</v>
       </c>
+      <c r="G180">
+        <v>5</v>
+      </c>
     </row>
     <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
@@ -6776,6 +6524,9 @@
       <c r="F181" t="s">
         <v>15</v>
       </c>
+      <c r="G181">
+        <v>5</v>
+      </c>
     </row>
     <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
@@ -7160,7 +6911,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
         <v>11</v>
       </c>
@@ -7558,15 +7309,21 @@
   </sheetData>
   <autoFilter ref="A1:K219" xr:uid="{2C036149-30B1-CB4A-9539-0B493FA5906D}">
     <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="2">
       <filters>
-        <filter val="Restoration - All restored to potential natural vegetation except for cropland and urban/builtup"/>
+        <filter val="Change"/>
+        <filter val="Diff"/>
       </filters>
     </filterColumn>
     <filterColumn colId="6">
       <filters>
-        <filter val="(just look to see how different)"/>
         <filter val="1st"/>
         <filter val="2nd"/>
+        <filter val="3rd"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K219">
@@ -7589,7 +7346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976F0BBF-6E1C-F84C-A5DE-45D3CC2FF64A}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" zoomScale="135" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="135" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -8242,10 +7999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CF352D-F6AF-504E-B4EA-B0B2D27DFF4C}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8254,7 +8011,7 @@
     <col min="2" max="2" width="134" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -8262,7 +8019,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>562</v>
       </c>
@@ -8270,7 +8027,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>564</v>
       </c>
@@ -8278,7 +8035,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -8286,7 +8043,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>567</v>
       </c>
@@ -8294,473 +8051,261 @@
         <v>568</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>570</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>571</v>
-      </c>
-      <c r="C8" t="s">
-        <v>572</v>
-      </c>
-      <c r="D8" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="C9" t="s">
-        <v>572</v>
-      </c>
-      <c r="D9" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>578</v>
-      </c>
-      <c r="C10" t="s">
-        <v>579</v>
-      </c>
-      <c r="D10" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>580</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>581</v>
-      </c>
-      <c r="C11" t="s">
-        <v>582</v>
-      </c>
-      <c r="D11" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>585</v>
-      </c>
-      <c r="C15" t="s">
-        <v>572</v>
-      </c>
-      <c r="D15" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>586</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>587</v>
-      </c>
-      <c r="C16" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>588</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="C17" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>590</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="C18" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B19" s="5" t="s">
-        <v>593</v>
-      </c>
-      <c r="C19" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>594</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="C20" t="s">
-        <v>596</v>
-      </c>
-      <c r="D20" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>598</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>599</v>
-      </c>
-      <c r="C21" t="s">
-        <v>600</v>
-      </c>
-      <c r="D21" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>601</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>602</v>
-      </c>
-      <c r="C22" t="s">
-        <v>582</v>
-      </c>
-      <c r="D22" t="s">
-        <v>603</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1" xr:uid="{EBB8C748-76B9-4043-9282-D63040408B16}"/>
-    <hyperlink ref="A17" r:id="rId2" xr:uid="{823512DE-11E4-9C47-B101-D2731DD63247}"/>
-    <hyperlink ref="A8" r:id="rId3" xr:uid="{40D583BD-6614-674E-B59A-8EFEAD50246A}"/>
-    <hyperlink ref="A9" r:id="rId4" xr:uid="{18E2467C-EE23-F543-AEA1-86E0A04A2612}"/>
-    <hyperlink ref="A11" r:id="rId5" xr:uid="{0CA6CEBF-CF66-EC47-9258-81FA57B13FE3}"/>
-    <hyperlink ref="A15" r:id="rId6" xr:uid="{00A3EB04-7C5F-1A49-A003-FCCC1D5008A9}"/>
-    <hyperlink ref="A20" r:id="rId7" xr:uid="{266C1E12-0D33-C04F-8ADC-900398A20DA1}"/>
-    <hyperlink ref="A21" r:id="rId8" xr:uid="{AE6F4ADE-E0AF-E341-916E-5D298385A83B}"/>
-    <hyperlink ref="A22" r:id="rId9" xr:uid="{CCCAAA1F-B6A3-9D4B-9BBB-BFE68E9ADBA3}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69C86BF5-2532-9C43-9803-F2FF107400AA}">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E1307C-A491-3A48-BEE2-6F0190788479}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B33" activeCellId="1" sqref="I27 B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>604</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>605</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>606</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>607</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>608</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>610</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F2" s="7" t="s">
-        <v>612</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>613</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>615</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>616</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>617</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F3" s="7" t="s">
-        <v>619</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>620</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>621</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>622</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>623</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>625</v>
-      </c>
-      <c r="B4" t="s">
-        <v>626</v>
+        <v>570</v>
+      </c>
+      <c r="B1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>572</v>
+      </c>
+      <c r="B3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1992</v>
       </c>
       <c r="C4" t="s">
-        <v>627</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>628</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>629</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>630</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>631</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>632</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>633</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>635</v>
-      </c>
-      <c r="C5" t="s">
-        <v>636</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>638</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>639</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>641</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>644</v>
-      </c>
-      <c r="C6" t="s">
-        <v>645</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>646</v>
-      </c>
-      <c r="G6" s="8">
-        <v>2020</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>647</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>648</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>650</v>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>1995</v>
       </c>
       <c r="C7" t="s">
-        <v>651</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>652</v>
-      </c>
-      <c r="G7" s="8">
-        <v>2020</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>632</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>617</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>653</v>
-      </c>
-      <c r="C8" t="s">
-        <v>654</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>655</v>
-      </c>
-      <c r="G8" s="8">
-        <v>2017</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>656</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>631</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>632</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>657</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>659</v>
-      </c>
-      <c r="C9" t="s">
-        <v>660</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>661</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>662</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>614</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>631</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>663</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>664</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>666</v>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>1998</v>
       </c>
       <c r="C10" t="s">
-        <v>667</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="9" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
-        <v>669</v>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>2001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>2004</v>
+      </c>
+      <c r="C16" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>2007</v>
+      </c>
+      <c r="C19" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>2010</v>
+      </c>
+      <c r="C22" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>2012</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>2013</v>
+      </c>
+      <c r="C25" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>2015</v>
+      </c>
+      <c r="C27" t="s">
+        <v>574</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>